<commit_message>
Incident and Weekly report completed
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/reportTemplates/MilestoneReportTemplate.xlsx
+++ b/src/main/resources/templates/reportTemplates/MilestoneReportTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OF\VNPT\DOC\Form báo cáo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OF\VNPT\myPlugin\plugin\reportPlugin\src\main\resources\templates\reportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Project Type</t>
   </si>
@@ -54,13 +54,62 @@
   </si>
   <si>
     <t>Milestone name</t>
+  </si>
+  <si>
+    <t>MILESTONE REPORT</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Báo cáo liệt kê danh sách các version của dự án. Lọc theo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Project Type, project category, project name, version status, start date và release date của version</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;Software&gt;</t>
+  </si>
+  <si>
+    <t>Quy Trinh</t>
+  </si>
+  <si>
+    <t>Du an 1</t>
+  </si>
+  <si>
+    <t>tên version</t>
+  </si>
+  <si>
+    <t>version status</t>
+  </si>
+  <si>
+    <t>&lt;Ngày bắt đầu dự kiến&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Ngày kết thúc dự kiến&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Ngày khai Timesheet cuối của issue thuộc version&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Ngày khai Timesheet đầu tiên của issue thuộc version&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mmm/yyyy"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,8 +125,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -87,6 +152,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -103,10 +174,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,84 +488,140 @@
     <col min="3" max="3" width="24.28515625" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" customWidth="1"/>
     <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="9" width="18.140625" customWidth="1"/>
+    <col min="6" max="9" width="18.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+    </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <f ca="1">NOW()</f>
+        <v>43116.617311458336</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>7</v>
+    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>